<commit_message>
add the sort for the crashes
</commit_message>
<xml_diff>
--- a/recode/afl_aflgo_compare.xlsx
+++ b/recode/afl_aflgo_compare.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>input</t>
   </si>
@@ -28,6 +28,7 @@
         <sz val="11"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">个</t>
     </r>
@@ -45,6 +46,7 @@
         <sz val="11"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">和”</t>
     </r>
@@ -76,9 +78,22 @@
         <sz val="11"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">全目标</t>
     </r>
+  </si>
+  <si>
+    <t>extendion_num</t>
+  </si>
+  <si>
+    <t>时间</t>
+  </si>
+  <si>
+    <t>240mini</t>
+  </si>
+  <si>
+    <t>引擎数量</t>
   </si>
   <si>
     <t>二进制名称</t>
@@ -345,6 +360,7 @@
       <sz val="11"/>
       <name val="Droid Sans Fallback"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -427,10 +443,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -464,93 +480,69 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4" t="n">
-        <f aca="false">D5-E5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <f aca="false">D6-E6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4" t="n">
-        <f aca="false">D7-E7</f>
-        <v>0</v>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>0</v>
@@ -569,7 +561,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0</v>
@@ -588,7 +580,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>0</v>
@@ -607,7 +599,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>0</v>
@@ -626,7 +618,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>0</v>
@@ -645,7 +637,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0</v>
@@ -664,7 +656,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0</v>
@@ -683,7 +675,7 @@
     </row>
     <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>0</v>
@@ -702,7 +694,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0</v>
@@ -721,10 +713,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2" t="n">
@@ -740,10 +732,10 @@
     </row>
     <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="2" t="n">
@@ -759,10 +751,10 @@
     </row>
     <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="2" t="n">
@@ -778,7 +770,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>7</v>
@@ -797,7 +789,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>7</v>
@@ -816,7 +808,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>7</v>
@@ -835,7 +827,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>7</v>
@@ -854,7 +846,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>7</v>
@@ -873,7 +865,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>7</v>
@@ -892,7 +884,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>7</v>
@@ -911,10 +903,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="2" t="n">
@@ -930,10 +922,10 @@
     </row>
     <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="2" t="n">
@@ -949,45 +941,45 @@
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>11626.51</v>
+        <v>0</v>
       </c>
       <c r="F29" s="4" t="n">
         <f aca="false">D29-E29</f>
-        <v>-11626.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>14</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="2" t="n">
-        <v>164.26</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1" t="n">
-        <v>165.72</v>
+        <v>0</v>
       </c>
       <c r="F30" s="4" t="n">
         <f aca="false">D30-E30</f>
-        <v>-1.46000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>14</v>
@@ -1006,83 +998,83 @@
     </row>
     <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>14</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="2" t="n">
-        <v>1153.73</v>
+        <v>0</v>
       </c>
       <c r="E32" s="1" t="n">
-        <v>7176.79</v>
+        <v>11626.51</v>
       </c>
       <c r="F32" s="4" t="n">
         <f aca="false">D32-E32</f>
-        <v>-6023.06</v>
+        <v>-11626.51</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>14</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="2" t="n">
-        <v>0</v>
+        <v>164.26</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>0</v>
+        <v>165.72</v>
       </c>
       <c r="F33" s="4" t="n">
         <f aca="false">D33-E33</f>
-        <v>0</v>
+        <v>-1.46000000000001</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>14</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="2" t="n">
-        <v>10110.25</v>
+        <v>0</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>748.26</v>
+        <v>0</v>
       </c>
       <c r="F34" s="4" t="n">
         <f aca="false">D34-E34</f>
-        <v>9361.99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>14</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="2" t="n">
-        <v>0</v>
+        <v>1153.73</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>0</v>
+        <v>7176.79</v>
       </c>
       <c r="F35" s="4" t="n">
         <f aca="false">D35-E35</f>
-        <v>0</v>
+        <v>-6023.06</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>14</v>
@@ -1101,302 +1093,302 @@
     </row>
     <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>14</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="2" t="n">
-        <v>2686.84</v>
+        <v>10110.25</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>5311.44</v>
+        <v>748.26</v>
       </c>
       <c r="F37" s="4" t="n">
         <f aca="false">D37-E37</f>
-        <v>-2624.6</v>
+        <v>9361.99</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="2" t="n">
-        <v>10.53</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>37.7</v>
+        <v>0</v>
       </c>
       <c r="F38" s="4" t="n">
         <f aca="false">D38-E38</f>
-        <v>-27.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="2" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F39" s="4" t="n">
         <f aca="false">D39-E39</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="2" t="n">
-        <v>53.68</v>
+        <v>2686.84</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>50.95</v>
+        <v>5311.44</v>
       </c>
       <c r="F40" s="4" t="n">
         <f aca="false">D40-E40</f>
-        <v>2.73</v>
+        <v>-2624.6</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="2" t="n">
-        <v>2.17</v>
+        <v>10.53</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>1.7</v>
+        <v>37.7</v>
       </c>
       <c r="F41" s="4" t="n">
         <f aca="false">D41-E41</f>
-        <v>0.47</v>
+        <v>-27.17</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="2" t="n">
-        <v>5.11</v>
+        <v>22</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>33.29</v>
+        <v>21</v>
       </c>
       <c r="F42" s="4" t="n">
         <f aca="false">D42-E42</f>
-        <v>-28.18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="2" t="n">
-        <v>35.94</v>
+        <v>53.68</v>
       </c>
       <c r="E43" s="1" t="n">
-        <v>39.85</v>
+        <v>50.95</v>
       </c>
       <c r="F43" s="4" t="n">
         <f aca="false">D43-E43</f>
-        <v>-3.91</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="2" t="n">
-        <v>17.52</v>
+        <v>2.17</v>
       </c>
       <c r="E44" s="1" t="n">
-        <v>9.3</v>
+        <v>1.7</v>
       </c>
       <c r="F44" s="4" t="n">
         <f aca="false">D44-E44</f>
-        <v>8.22</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="2" t="n">
-        <v>4544.27</v>
+        <v>5.11</v>
       </c>
       <c r="E45" s="1" t="n">
-        <v>1116.49</v>
+        <v>33.29</v>
       </c>
       <c r="F45" s="4" t="n">
         <f aca="false">D45-E45</f>
-        <v>3427.78</v>
+        <v>-28.18</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="2" t="n">
-        <v>808.24</v>
+        <v>35.94</v>
       </c>
       <c r="E46" s="1" t="n">
-        <v>1592.53</v>
+        <v>39.85</v>
       </c>
       <c r="F46" s="4" t="n">
         <f aca="false">D46-E46</f>
-        <v>-784.29</v>
+        <v>-3.91</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="2" t="n">
-        <v>19.18</v>
+        <v>17.52</v>
       </c>
       <c r="E47" s="1" t="n">
-        <v>19.55</v>
+        <v>9.3</v>
       </c>
       <c r="F47" s="4" t="n">
         <f aca="false">D47-E47</f>
-        <v>-0.370000000000001</v>
+        <v>8.22</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="2" t="n">
-        <v>930.52</v>
+        <v>4544.27</v>
       </c>
       <c r="E48" s="1" t="n">
-        <v>617.85</v>
+        <v>1116.49</v>
       </c>
       <c r="F48" s="4" t="n">
         <f aca="false">D48-E48</f>
-        <v>312.67</v>
+        <v>3427.78</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="2" t="n">
-        <v>0</v>
+        <v>808.24</v>
       </c>
       <c r="E49" s="1" t="n">
-        <v>0</v>
+        <v>1592.53</v>
       </c>
       <c r="F49" s="4" t="n">
         <f aca="false">D49-E49</f>
-        <v>0</v>
+        <v>-784.29</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="2" t="n">
-        <v>0</v>
+        <v>19.18</v>
       </c>
       <c r="E50" s="1" t="n">
-        <v>0</v>
+        <v>19.55</v>
       </c>
       <c r="F50" s="4" t="n">
         <f aca="false">D50-E50</f>
-        <v>0</v>
+        <v>-0.370000000000001</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="2" t="n">
-        <v>12.53</v>
+        <v>930.52</v>
       </c>
       <c r="E51" s="1" t="n">
-        <v>15.8</v>
+        <v>617.85</v>
       </c>
       <c r="F51" s="4" t="n">
         <f aca="false">D51-E51</f>
-        <v>-3.27</v>
+        <v>312.67</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="2" t="n">
-        <v>1.07</v>
+        <v>0</v>
       </c>
       <c r="E52" s="1" t="n">
-        <v>1.07</v>
+        <v>0</v>
       </c>
       <c r="F52" s="4" t="n">
         <f aca="false">D52-E52</f>
@@ -1405,178 +1397,178 @@
     </row>
     <row r="53" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="2" t="n">
-        <v>659.48</v>
+        <v>0</v>
       </c>
       <c r="E53" s="1" t="n">
-        <v>631.47</v>
+        <v>0</v>
       </c>
       <c r="F53" s="4" t="n">
         <f aca="false">D53-E53</f>
-        <v>28.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="2" t="n">
-        <v>1.8</v>
+        <v>12.53</v>
       </c>
       <c r="E54" s="1" t="n">
-        <v>0.45</v>
+        <v>15.8</v>
       </c>
       <c r="F54" s="4" t="n">
         <f aca="false">D54-E54</f>
-        <v>1.35</v>
+        <v>-3.27</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B55" s="1" t="n">
         <v>28</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="2" t="n">
-        <v>2091.13</v>
+        <v>1.07</v>
       </c>
       <c r="E55" s="1" t="n">
-        <v>1735.54</v>
+        <v>1.07</v>
       </c>
       <c r="F55" s="4" t="n">
         <f aca="false">D55-E55</f>
-        <v>355.59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B56" s="1" t="n">
         <v>28</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="2" t="n">
-        <v>118.15</v>
+        <v>659.48</v>
       </c>
       <c r="E56" s="1" t="n">
-        <v>18.39</v>
+        <v>631.47</v>
       </c>
       <c r="F56" s="4" t="n">
         <f aca="false">D56-E56</f>
-        <v>99.76</v>
+        <v>28.01</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B57" s="1" t="n">
         <v>28</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="2" t="n">
-        <v>1.12</v>
+        <v>1.8</v>
       </c>
       <c r="E57" s="1" t="n">
-        <v>1.72</v>
+        <v>0.45</v>
       </c>
       <c r="F57" s="4" t="n">
         <f aca="false">D57-E57</f>
-        <v>-0.6</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B58" s="1" t="n">
         <v>28</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="2" t="n">
-        <v>0</v>
+        <v>2091.13</v>
       </c>
       <c r="E58" s="1" t="n">
-        <v>0</v>
+        <v>1735.54</v>
       </c>
       <c r="F58" s="4" t="n">
         <f aca="false">D58-E58</f>
-        <v>0</v>
+        <v>355.59</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B59" s="1" t="n">
         <v>28</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="2" t="n">
-        <v>0</v>
+        <v>118.15</v>
       </c>
       <c r="E59" s="1" t="n">
-        <v>0</v>
+        <v>18.39</v>
       </c>
       <c r="F59" s="4" t="n">
         <f aca="false">D59-E59</f>
-        <v>0</v>
+        <v>99.76</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B60" s="1" t="n">
         <v>28</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="2" t="n">
-        <v>1.4</v>
+        <v>1.12</v>
       </c>
       <c r="E60" s="1" t="n">
-        <v>1.25</v>
+        <v>1.72</v>
       </c>
       <c r="F60" s="4" t="n">
         <f aca="false">D60-E60</f>
-        <v>0.15</v>
+        <v>-0.6</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B61" s="1" t="n">
         <v>28</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="2" t="n">
-        <v>1.93</v>
+        <v>0</v>
       </c>
       <c r="E61" s="1" t="n">
-        <v>0.53</v>
+        <v>0</v>
       </c>
       <c r="F61" s="4" t="n">
         <f aca="false">D61-E61</f>
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B62" s="1" t="n">
         <v>28</v>
@@ -1595,45 +1587,49 @@
     </row>
     <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B63" s="1" t="n">
         <v>28</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="2" t="n">
-        <v>1.77</v>
+        <v>1.4</v>
       </c>
       <c r="E63" s="1" t="n">
-        <v>1.8</v>
+        <v>1.25</v>
       </c>
       <c r="F63" s="4" t="n">
         <f aca="false">D63-E63</f>
-        <v>-0.03</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="B64" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="C64" s="4"/>
       <c r="D64" s="2" t="n">
-        <v>1792</v>
+        <v>1.93</v>
       </c>
       <c r="E64" s="1" t="n">
-        <v>10527</v>
-      </c>
-      <c r="F64" s="1" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="F64" s="4" t="n">
         <f aca="false">D64-E64</f>
-        <v>-8735</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="B65" s="1" t="n">
+        <v>28</v>
+      </c>
       <c r="C65" s="4"/>
       <c r="D65" s="2" t="n">
         <v>0</v>
@@ -1648,58 +1644,60 @@
     </row>
     <row r="66" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B66" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="B66" s="1" t="n">
+        <v>28</v>
+      </c>
       <c r="C66" s="4"/>
       <c r="D66" s="2" t="n">
-        <v>0</v>
+        <v>1.77</v>
       </c>
       <c r="E66" s="1" t="n">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="F66" s="4" t="n">
         <f aca="false">D66-E66</f>
-        <v>0</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B67" s="1"/>
-      <c r="C67" s="4"/>
+      <c r="C67" s="1"/>
       <c r="D67" s="2" t="n">
-        <v>0</v>
+        <v>1792</v>
       </c>
       <c r="E67" s="1" t="n">
-        <v>762.67</v>
-      </c>
-      <c r="F67" s="4" t="n">
+        <v>10527</v>
+      </c>
+      <c r="F67" s="1" t="n">
         <f aca="false">D67-E67</f>
-        <v>-762.67</v>
+        <v>-8735</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="4"/>
       <c r="D68" s="2" t="n">
-        <v>6634.04</v>
+        <v>0</v>
       </c>
       <c r="E68" s="1" t="n">
-        <v>843.66</v>
+        <v>0</v>
       </c>
       <c r="F68" s="4" t="n">
         <f aca="false">D68-E68</f>
-        <v>5790.38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="4"/>
@@ -1716,41 +1714,41 @@
     </row>
     <row r="70" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="4"/>
       <c r="D70" s="2" t="n">
-        <v>309.19</v>
+        <v>0</v>
       </c>
       <c r="E70" s="1" t="n">
-        <v>5756.43</v>
+        <v>762.67</v>
       </c>
       <c r="F70" s="4" t="n">
         <f aca="false">D70-E70</f>
-        <v>-5447.24</v>
+        <v>-762.67</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="4"/>
       <c r="D71" s="2" t="n">
-        <v>1690.76</v>
+        <v>6634.04</v>
       </c>
       <c r="E71" s="1" t="n">
-        <v>0</v>
+        <v>843.66</v>
       </c>
       <c r="F71" s="4" t="n">
         <f aca="false">D71-E71</f>
-        <v>1690.76</v>
+        <v>5790.38</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="4"/>
@@ -1767,148 +1765,72 @@
     </row>
     <row r="73" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="4"/>
       <c r="D73" s="2" t="n">
-        <v>5177.17</v>
+        <v>309.19</v>
       </c>
       <c r="E73" s="1" t="n">
-        <v>2065.08</v>
+        <v>5756.43</v>
       </c>
       <c r="F73" s="4" t="n">
         <f aca="false">D73-E73</f>
+        <v>-5447.24</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="2" t="n">
+        <v>1690.76</v>
+      </c>
+      <c r="E74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" s="4" t="n">
+        <f aca="false">D74-E74</f>
+        <v>1690.76</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" s="1"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" s="4" t="n">
+        <f aca="false">D75-E75</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="2" t="n">
+        <v>5177.17</v>
+      </c>
+      <c r="E76" s="1" t="n">
+        <v>2065.08</v>
+      </c>
+      <c r="F76" s="4" t="n">
+        <f aca="false">D76-E76</f>
         <v>3112.09</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="109" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="116" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="118" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="119" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="120" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="121" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="122" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="123" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="124" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="125" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="126" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="127" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="128" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="129" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="130" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="131" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="132" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="134" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="135" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="136" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="137" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="138" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="142" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="143" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="144" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="145" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="146" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="147" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="148" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="149" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="155" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="156" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="162" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="163" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="165" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="166" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="167" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="169" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="170" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="172" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="173" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="174" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="175" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="176" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="177" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="184" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="185" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="186" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="187" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="188" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="189" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="190" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="191" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="193" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="194" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="195" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="196" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="197" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="198" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="199" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="200" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>